<commit_message>
Modified every Hunter skills description to fit the new standard.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\Hunter\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\Done\2_Hunter\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
   <si>
     <t>Additional Info</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Summon an Distortion Area (3 turns)</t>
   </si>
   <si>
-    <t>Disclaimer: Can't fix your horrible voice sound…</t>
-  </si>
-  <si>
     <t>Shockwave Arrow</t>
   </si>
   <si>
@@ -104,15 +101,6 @@
     <t>Push 2 cells in the opposite direction of the spell cast point.</t>
   </si>
   <si>
-    <t>If is an enemy, [[Damage:  25-30 wind ]]</t>
-  </si>
-  <si>
-    <t>Your prey will flee!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An hunter using a shockwave?!? Are you nuts? </t>
-  </si>
-  <si>
     <t>Glowing Arrow</t>
   </si>
   <si>
@@ -125,9 +113,6 @@
     <t>On Distortion Area: [[Area of effect: - 8 Singles cells]]</t>
   </si>
   <si>
-    <t>On Distortion Area: [[Area of effect: - 4 Singles cells]]</t>
-  </si>
-  <si>
     <t>From the distortion Area, shoot on the 4 lines and 4 diagonals.</t>
   </si>
   <si>
@@ -137,18 +122,9 @@
     <t>If is an enemy, [[Damage:  15-20 light ]]</t>
   </si>
   <si>
-    <t>On target: [[Reduce range by 1]] (2 turns)</t>
-  </si>
-  <si>
     <t>On Distortion Area: If is player team, [[Heal:  15-20 light ]]</t>
   </si>
   <si>
-    <t>be reconforting with its warmness.</t>
-  </si>
-  <si>
-    <t>The utmost of versatility. Can blind or either</t>
-  </si>
-  <si>
     <t>Piercing Arrow</t>
   </si>
   <si>
@@ -161,15 +137,6 @@
     <t>Map obstacle reduct damage too.</t>
   </si>
   <si>
-    <t>Damage exemple: (50,40,30,20,10,0,0,0…..)</t>
-  </si>
-  <si>
-    <t>[[Damage:  (50 - (20% per obstacle crossed)) earth ]]</t>
-  </si>
-  <si>
-    <t>I'll hunt you down to your lair if I need to.</t>
-  </si>
-  <si>
     <t>[[Range: 2-00 ]]</t>
   </si>
   <si>
@@ -200,12 +167,6 @@
     <t>Burning Ground (3 turns)</t>
   </si>
   <si>
-    <t>I'm willing to do ANYTHING to catch you, even if its</t>
-  </si>
-  <si>
-    <t>means burning to the ground the landscape!</t>
-  </si>
-  <si>
     <t>Cursed Arrow</t>
   </si>
   <si>
@@ -242,9 +203,6 @@
     <t>Poison Arrow</t>
   </si>
   <si>
-    <t>If I have to sacrifice myself to eliminate you, so be it</t>
-  </si>
-  <si>
     <t>[[Max effect accumulation: 3 ]]</t>
   </si>
   <si>
@@ -266,15 +224,6 @@
     <t>Effect name: ''Poison''.</t>
   </si>
   <si>
-    <t>Hidden in the darkness, I'll watch your life</t>
-  </si>
-  <si>
-    <t>leave your body slowly, but surely.</t>
-  </si>
-  <si>
-    <t>The hunter has become the prey, irony of fate…</t>
-  </si>
-  <si>
     <t>Survival</t>
   </si>
   <si>
@@ -317,24 +266,15 @@
     <t>Usable only If not under ''Treason'' effect</t>
   </si>
   <si>
-    <t>Probably the only living thing that appreciate you.</t>
-  </si>
-  <si>
     <t>Infected Bite</t>
   </si>
   <si>
-    <t>An infected bite, as if being bitten wasn't enough.</t>
-  </si>
-  <si>
     <t>[[Range: 1 ]]</t>
   </si>
   <si>
     <t>[[Max effect accumulation: 2 ]]</t>
   </si>
   <si>
-    <t>[[Damage:  5-10 earth ]]                                                      [[Damage:  20 dark ]] (2 turns)</t>
-  </si>
-  <si>
     <t>The poison damage are triggered at the start of the target turn.</t>
   </si>
   <si>
@@ -359,10 +299,55 @@
     <t>[[Number of turns between two casts: 00 ]]</t>
   </si>
   <si>
-    <t>It's you or me, sorry buddy.</t>
-  </si>
-  <si>
     <t>Canis Lupus skill</t>
+  </si>
+  <si>
+    <t>Summons a Distortion Area.</t>
+  </si>
+  <si>
+    <t>If is an enemy, [[Damage:  25-30 air ]]</t>
+  </si>
+  <si>
+    <t>On Distortion Area: [[Area of effect: - 3 Singles cells]]</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage on enemies and push the target.           When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage on enemies. When targeting an enemy, reduce range.                                                                                 When targeting the Distortion Area, the skill is replicated on each straight and diagonal line of the Distortion Area and heal caster and allies when touching them.</t>
+  </si>
+  <si>
+    <t>If is an enemy, [[Reduce range by 1]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Damage:  (50 - (10 * obstacle crossed)) earth ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage. Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage on impact and Fire-type damage on the burning area. The burning area dealt damage for every burning cell crossed.</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage if not under Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage. If not under Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
+  </si>
+  <si>
+    <t>Poisons that inflicts Dark-type damage. The poison last longer if the caster is under Blood Mark effect.</t>
+  </si>
+  <si>
+    <t>Increases the caster HP and MP temporarily. Can only be used when the caster is low on HP.</t>
+  </si>
+  <si>
+    <t>[[Damage: 5-10 earth ]]                                                      [[Damage: 20 dark ]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Summons a Canis Lupus which poison the enemies. Can only be used if the caster is not under the Treason effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage and give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <t>Heal the caster but unsummon the Canis Lupus and preven from summoning it for the rest of the fight. Can only be used when targeting the caster Canis Lupus.</t>
   </si>
 </sst>
 </file>
@@ -542,9 +527,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -570,6 +552,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +904,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1029,14 +1014,14 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="1"/>
@@ -1077,7 +1062,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1086,10 +1071,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>108</v>
+      <c r="C5" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1108,14 +1093,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1127,7 +1112,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1139,14 +1124,14 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1170,21 +1155,21 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1213,15 +1198,15 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10" t="s">
-        <v>102</v>
+      <c r="C26" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>103</v>
+      <c r="C27" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1238,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="G13" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1246,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1270,48 +1255,48 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
+      <c r="C5" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1324,102 +1309,95 @@
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1429,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1430,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1461,23 +1439,23 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
+      <c r="C5" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
@@ -1489,154 +1467,147 @@
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B30" s="1"/>
-      <c r="C30" s="11" t="s">
-        <v>31</v>
+      <c r="C30" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1646,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1640,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1678,10 +1649,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
+      <c r="C5" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1700,7 +1671,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1712,21 +1683,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1738,7 +1709,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1750,7 +1721,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1762,7 +1733,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1791,22 +1762,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="10" t="s">
-        <v>41</v>
+      <c r="C24" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1816,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1803,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1848,156 +1812,149 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
+      <c r="C5" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>52</v>
+      <c r="C20" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="13" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2010,7 +1967,7 @@
   <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,7 +1987,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2039,10 +1996,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>69</v>
+      <c r="C5" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2054,14 +2011,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2080,7 +2037,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -2106,7 +2063,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2118,7 +2075,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2129,29 +2086,29 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="13" t="s">
-        <v>65</v>
+      <c r="C19" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="15" t="s">
-        <v>64</v>
+      <c r="C20" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="14" t="s">
-        <v>63</v>
+      <c r="C21" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2180,15 +2137,15 @@
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="10" t="s">
-        <v>62</v>
+      <c r="C28" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
-        <v>67</v>
+      <c r="C29" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -2205,10 +2162,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D31"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,7 +2185,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2237,168 +2194,161 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>77</v>
+      <c r="C5" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
-        <v>76</v>
+      <c r="C29" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2431,7 +2381,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2440,10 +2390,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>79</v>
+      <c r="C5" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2455,14 +2405,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2474,7 +2424,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2486,14 +2436,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2517,14 +2467,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2553,15 +2503,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="10" t="s">
-        <v>86</v>
+      <c r="C24" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>87</v>
+      <c r="C25" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2580,8 +2530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H27" sqref="F1:H27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,8 +2547,8 @@
   <sheetData>
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
-      <c r="G1" s="16" t="s">
-        <v>109</v>
+      <c r="G1" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2613,12 +2563,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="8" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2630,15 +2580,15 @@
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
+      <c r="C5" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
-        <v>96</v>
+      <c r="G5" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2653,19 +2603,19 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2675,12 +2625,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="3" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2695,19 +2645,19 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -2722,7 +2672,7 @@
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -2737,7 +2687,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2774,13 +2724,13 @@
     </row>
     <row r="19" spans="2:8" ht="78" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="17" t="s">
-        <v>92</v>
+      <c r="C19" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="18" t="s">
-        <v>99</v>
+      <c r="G19" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2823,32 +2773,32 @@
     </row>
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>93</v>
+      <c r="C25" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="10" t="s">
-        <v>93</v>
+      <c r="G25" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="19"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26" s="20"/>
+      <c r="G26" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="19"/>
-      <c r="D27" s="21"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="20"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified all the Ninja skills descriptions to fit the new standard.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -871,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1225,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G13" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
@@ -1783,7 +1783,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,7 +2531,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Upgraded the Hunter skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
   <si>
     <t>Additional Info</t>
   </si>
@@ -62,12 +62,6 @@
     <t>[[Area of effect: - Single cell]]</t>
   </si>
   <si>
-    <t>Allow sight.</t>
-  </si>
-  <si>
-    <t>Block walk.</t>
-  </si>
-  <si>
     <t>Summon an Distortion Area (3 turns)</t>
   </si>
   <si>
@@ -92,12 +86,6 @@
     <t>On target: [[Area of effect: - Single cell]]</t>
   </si>
   <si>
-    <t>From the Distortion Area, the range of the skill is the distance of the hunter from the Distortion Area.</t>
-  </si>
-  <si>
-    <t>The first obstacle encountered stop the skill progression.</t>
-  </si>
-  <si>
     <t>Push 2 cells in the opposite direction of the spell cast point.</t>
   </si>
   <si>
@@ -113,18 +101,9 @@
     <t>On Distortion Area: [[Area of effect: - 8 Singles cells]]</t>
   </si>
   <si>
-    <t>From the distortion Area, shoot on the 4 lines and 4 diagonals.</t>
-  </si>
-  <si>
     <t>[[Range: 4-8 ]]</t>
   </si>
   <si>
-    <t>If is an enemy, [[Damage:  15-20 light ]]</t>
-  </si>
-  <si>
-    <t>On Distortion Area: If is player team, [[Heal:  15-20 light ]]</t>
-  </si>
-  <si>
     <t>Piercing Arrow</t>
   </si>
   <si>
@@ -134,9 +113,6 @@
     <t>[[Area of effect: - Stright line to the end of the map]]</t>
   </si>
   <si>
-    <t>Map obstacle reduct damage too.</t>
-  </si>
-  <si>
     <t>[[Range: 2-00 ]]</t>
   </si>
   <si>
@@ -161,9 +137,6 @@
     <t>Impact: [[Damage:  20-30 light ]]</t>
   </si>
   <si>
-    <t>The Burning Ground damage are triggered at the start of a target turn on the area and for each of its moving into a burning cell.</t>
-  </si>
-  <si>
     <t>Burning Ground (3 turns)</t>
   </si>
   <si>
@@ -197,9 +170,6 @@
     <t>If under ''Blood Mark'' effect: [[Damage: 75 fire + 75 dark ]]</t>
   </si>
   <si>
-    <t>Self: If under ''Blood Mark'' effect, Unbuff ''Blood Mark'' effect.</t>
-  </si>
-  <si>
     <t>Poison Arrow</t>
   </si>
   <si>
@@ -245,9 +215,6 @@
     <t>Effect name: ''Survival''.</t>
   </si>
   <si>
-    <t>Usable only if has 25% or less HP.</t>
-  </si>
-  <si>
     <t>Canis Lupus</t>
   </si>
   <si>
@@ -263,9 +230,6 @@
     <t>Summon a ''Canis Lupus'' [[25% of hunter max HP, 5 AP, 5 MP, 30% earth resistence, -10% fire resistence, -30% water resistence, 10% air resistence, -30% light resistence, 30% dark resistence]]</t>
   </si>
   <si>
-    <t>Usable only If not under ''Treason'' effect</t>
-  </si>
-  <si>
     <t>Infected Bite</t>
   </si>
   <si>
@@ -275,21 +239,12 @@
     <t>[[Max effect accumulation: 2 ]]</t>
   </si>
   <si>
-    <t>The poison damage are triggered at the start of the target turn.</t>
-  </si>
-  <si>
     <t>Last Resort</t>
   </si>
   <si>
     <t>Effect name: ''Treason''.</t>
   </si>
   <si>
-    <t>Can only target ''Canis Lupus''.</t>
-  </si>
-  <si>
-    <t>Self: [[Heal:  The max HP of ''Canis Lupus'' ]]</t>
-  </si>
-  <si>
     <t>Self: [[Treason effect ]] (00 turns)</t>
   </si>
   <si>
@@ -302,52 +257,61 @@
     <t>Canis Lupus skill</t>
   </si>
   <si>
-    <t>Summons a Distortion Area.</t>
-  </si>
-  <si>
-    <t>If is an enemy, [[Damage:  25-30 air ]]</t>
-  </si>
-  <si>
     <t>On Distortion Area: [[Area of effect: - 3 Singles cells]]</t>
   </si>
   <si>
-    <t>Inflicts Air-type damage on enemies and push the target.           When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.</t>
-  </si>
-  <si>
-    <t>Inflicts Light-type damage on enemies. When targeting an enemy, reduce range.                                                                                 When targeting the Distortion Area, the skill is replicated on each straight and diagonal line of the Distortion Area and heal caster and allies when touching them.</t>
-  </si>
-  <si>
-    <t>If is an enemy, [[Reduce range by 1]] (2 turns)</t>
-  </si>
-  <si>
     <t>[[Damage:  (50 - (10 * obstacle crossed)) earth ]]</t>
   </si>
   <si>
-    <t>Inflicts Light-type damage. Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
-  </si>
-  <si>
-    <t>Inflicts Light-type damage on impact and Fire-type damage on the burning area. The burning area dealt damage for every burning cell crossed.</t>
-  </si>
-  <si>
-    <t>Inflicts Fire-type damage if not under Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage. If not under Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
-  </si>
-  <si>
-    <t>Poisons that inflicts Dark-type damage. The poison last longer if the caster is under Blood Mark effect.</t>
-  </si>
-  <si>
-    <t>Increases the caster HP and MP temporarily. Can only be used when the caster is low on HP.</t>
-  </si>
-  <si>
     <t>[[Damage: 5-10 earth ]]                                                      [[Damage: 20 dark ]] (2 turns)</t>
   </si>
   <si>
-    <t>Summons a Canis Lupus which poison the enemies. Can only be used if the caster is not under the Treason effect.</t>
-  </si>
-  <si>
     <t>Inflicts Earth-type damage and give poisons that inflicts Dark-type damage.</t>
   </si>
   <si>
-    <t>Heal the caster but unsummon the Canis Lupus and preven from summoning it for the rest of the fight. Can only be used when targeting the caster Canis Lupus.</t>
+    <t>Summons a Distortion Area that dosn't block the field of view.  Affect other skills of the caster.</t>
+  </si>
+  <si>
+    <t>[[Damage:  25-30 air ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage on enemies.                                             Push the target.                                                                              When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.     The first obstacle encountered stop the skill progression.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage on enemies.                                        Reduce range of enemies.                                                                                 When targeting the Distortion Area, the skill is replicated on each straight and diagonal line of the Distortion Area and heal caster and allies when touching them.                                                               The first obstacle encountered stop the skill progression.</t>
+  </si>
+  <si>
+    <t>[[Damage:  15-20 light ]]</t>
+  </si>
+  <si>
+    <t>[[Reduce range by 1]] (2 turns)</t>
+  </si>
+  <si>
+    <t>From Distortion Area: [[Heal:  15-20 light ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage.                                                         Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage on impact and Fire-type damage on the burning area.                                                                                     The burning area dealt damage for every burning cell crossed.</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage if the caster isn't under Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage.                                             If the caster isn't under Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
+  </si>
+  <si>
+    <t>Poisons that inflicts Dark-type damage.                                           The poison last longer if the caster is under Blood Mark effect.</t>
+  </si>
+  <si>
+    <t>Increases the caster HP and MP temporarily.                                  Can only be used when the caster has 25% or less HP remaning.</t>
+  </si>
+  <si>
+    <t>Summons a Canis Lupus which poison the enemies.                      Can only be used if the caster is not under the Treason effect.</t>
+  </si>
+  <si>
+    <t>Heal the caster but unsummon the Canis Lupus and preven from summoning it for the rest of the fight.                                              Can only be used when targeting the caster Canis Lupus.</t>
+  </si>
+  <si>
+    <t>Self: [[Heal: The max HP of ''Canis Lupus'' ]]</t>
   </si>
 </sst>
 </file>
@@ -427,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -496,25 +460,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,12 +485,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,13 +494,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,20 +841,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>89</v>
+      <c r="C5" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -915,64 +865,64 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1"/>
@@ -984,8 +934,8 @@
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1002,7 +952,7 @@
     </row>
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="1"/>
@@ -1014,22 +964,13 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1039,10 +980,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,20 +1002,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>81</v>
+      <c r="C3" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>104</v>
+      <c r="C5" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1085,64 +1026,64 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>72</v>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>78</v>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>87</v>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>47</v>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1"/>
@@ -1154,22 +1095,22 @@
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>84</v>
+      <c r="C18" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>85</v>
+      <c r="C19" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>86</v>
+      <c r="C20" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1186,7 +1127,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="1"/>
@@ -1198,22 +1139,15 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="9" t="s">
-        <v>82</v>
+      <c r="C26" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1223,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G13" sqref="G12:G13"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,20 +1179,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>12</v>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>92</v>
+      <c r="C5" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1269,91 +1203,91 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>91</v>
+      <c r="C17" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>90</v>
+      <c r="C19" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>21</v>
+      <c r="C20" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1370,7 +1304,7 @@
     </row>
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="1"/>
@@ -1380,24 +1314,15 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,20 +1354,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>93</v>
+      <c r="C5" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1453,110 +1378,110 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>24</v>
+      <c r="C14" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>14</v>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>25</v>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>28</v>
+      <c r="C21" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>94</v>
+      <c r="C22" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
+      <c r="C23" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1573,7 +1498,7 @@
     </row>
     <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="1"/>
@@ -1585,29 +1510,13 @@
     </row>
     <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="C29" s="9"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1639,20 +1548,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>30</v>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>96</v>
+      <c r="C5" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1663,65 +1572,65 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>32</v>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1732,8 +1641,8 @@
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>95</v>
+      <c r="C18" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1750,7 +1659,7 @@
     </row>
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="1"/>
@@ -1762,15 +1671,13 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1783,7 +1690,7 @@
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,20 +1709,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>35</v>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>97</v>
+      <c r="C5" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1826,72 +1733,72 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>36</v>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1902,22 +1809,22 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="12" t="s">
-        <v>43</v>
+      <c r="C20" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="13" t="s">
-        <v>40</v>
+      <c r="C21" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1934,7 +1841,7 @@
     </row>
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="1"/>
@@ -1944,17 +1851,15 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1964,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,20 +1891,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>44</v>
+      <c r="C3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>98</v>
+      <c r="C5" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2010,72 +1915,72 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>46</v>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
+      <c r="C15" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
+      <c r="C17" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2086,29 +1991,29 @@
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>52</v>
+      <c r="C19" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>51</v>
+      <c r="C20" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="13" t="s">
-        <v>50</v>
+      <c r="C21" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2125,7 +2030,7 @@
     </row>
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="1"/>
@@ -2137,22 +2042,15 @@
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="9" t="s">
-        <v>49</v>
+      <c r="C28" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2162,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,20 +2082,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>55</v>
+      <c r="C3" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>99</v>
+      <c r="C5" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2208,83 +2106,83 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>59</v>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
-        <v>56</v>
+      <c r="C14" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>57</v>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>58</v>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1"/>
@@ -2296,15 +2194,15 @@
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
+      <c r="C21" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>61</v>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2321,7 +2219,7 @@
     </row>
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="1"/>
@@ -2333,22 +2231,15 @@
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="9" t="s">
-        <v>62</v>
+      <c r="C28" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2358,10 +2249,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,20 +2271,20 @@
     </row>
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>63</v>
+      <c r="C3" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>100</v>
+      <c r="C5" s="15" t="s">
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2404,57 +2295,57 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>66</v>
+      <c r="C12" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="7" t="s">
-        <v>47</v>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1"/>
@@ -2466,15 +2357,15 @@
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>68</v>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>67</v>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2491,7 +2382,7 @@
     </row>
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="1"/>
@@ -2503,22 +2394,15 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
-        <v>69</v>
+      <c r="C24" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2528,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H27"/>
+  <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,8 +2431,8 @@
   <sheetData>
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
-      <c r="G1" s="15" t="s">
-        <v>88</v>
+      <c r="G1" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2562,33 +2446,33 @@
     </row>
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>71</v>
+      <c r="C3" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="8" t="s">
-        <v>77</v>
+      <c r="G3" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="22" t="s">
-        <v>102</v>
+      <c r="C5" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="22" t="s">
-        <v>103</v>
+      <c r="G5" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2602,114 +2486,114 @@
     </row>
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>72</v>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>73</v>
+      <c r="C9" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="3" t="s">
-        <v>78</v>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="3" t="s">
-        <v>31</v>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="7" t="s">
-        <v>79</v>
+      <c r="G13" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>74</v>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="1"/>
@@ -2722,15 +2606,15 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" ht="78" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="16" t="s">
-        <v>75</v>
+      <c r="C19" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="17" t="s">
-        <v>101</v>
+      <c r="G19" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -2753,12 +2637,12 @@
     </row>
     <row r="23" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="1"/>
@@ -2773,32 +2657,19 @@
     </row>
     <row r="25" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="G25" s="8"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="19"/>
+      <c r="D26" s="13"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
-      <c r="D27" s="20"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="21"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>